<commit_message>
update DB structure to include seedlings table, type/variety fields in plant_type
</commit_message>
<xml_diff>
--- a/SampleData/SampleData.xlsx
+++ b/SampleData/SampleData.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Documents/GitHub/Harvester/SampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7B626A-93BC-CE45-B89B-7D40AEEC5706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3C6BB2-D56D-CB4F-98F8-90F66C95909D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32700" yWindow="4280" windowWidth="24200" windowHeight="20820" activeTab="4" xr2:uid="{2FC47D8B-67C3-324E-B295-947C478D14E9}"/>
+    <workbookView xWindow="35140" yWindow="3040" windowWidth="29400" windowHeight="22660" activeTab="5" xr2:uid="{2FC47D8B-67C3-324E-B295-947C478D14E9}"/>
   </bookViews>
   <sheets>
-    <sheet name="PlantMeasurements" sheetId="1" r:id="rId1"/>
-    <sheet name="Plants" sheetId="2" r:id="rId2"/>
+    <sheet name="SolutionReadings" sheetId="5" r:id="rId1"/>
+    <sheet name="PlantTypes" sheetId="4" r:id="rId2"/>
     <sheet name="SeedLots" sheetId="3" r:id="rId3"/>
-    <sheet name="PlantTypes" sheetId="4" r:id="rId4"/>
-    <sheet name="SolutionReadings" sheetId="5" r:id="rId5"/>
-    <sheet name="Harvester_SampleData_SolutionRe" sheetId="6" r:id="rId6"/>
+    <sheet name="Seedlings" sheetId="7" r:id="rId4"/>
+    <sheet name="Plants" sheetId="2" r:id="rId5"/>
+    <sheet name="PlantMeasurements" sheetId="1" r:id="rId6"/>
+    <sheet name="Harvester_SampleData_SolutionRe" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
-  <si>
-    <t>ReadingID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>PH</t>
   </si>
@@ -60,21 +58,6 @@
     <t>PlantTypeID</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>PlantingInstructions</t>
-  </si>
-  <si>
-    <t>SeedLotID</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -93,24 +76,6 @@
     <t>PlantID</t>
   </si>
   <si>
-    <t>StartDate</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>GerminationDate</t>
-  </si>
-  <si>
-    <t>GerminationFailure</t>
-  </si>
-  <si>
-    <t>TransferDate</t>
-  </si>
-  <si>
-    <t>PlantMeasurementID</t>
-  </si>
-  <si>
     <t>SizeX</t>
   </si>
   <si>
@@ -172,6 +137,42 @@
   </si>
   <si>
     <t>2022-04-15</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>variety</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>planting_instructions</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>germination_date</t>
+  </si>
+  <si>
+    <t>germination_failure</t>
+  </si>
+  <si>
+    <t>seed_lot_id</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>transfer_date</t>
+  </si>
+  <si>
+    <t>seedling_id</t>
   </si>
 </sst>
 </file>
@@ -538,80 +539,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9AFE0D-20AE-8C4F-9881-9960F9203F3B}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB536F2-B6F5-5D4C-A150-E99119632D93}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>800</v>
+      </c>
+      <c r="C2">
+        <v>8.5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6.1</v>
+      </c>
+      <c r="B3">
+        <v>810</v>
+      </c>
+      <c r="C3">
+        <v>8.4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>6.1</v>
+      </c>
+      <c r="B4">
+        <v>820</v>
+      </c>
+      <c r="C4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6.1</v>
+      </c>
+      <c r="B5">
+        <v>830</v>
+      </c>
+      <c r="C5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>6.2</v>
+      </c>
+      <c r="B6">
+        <v>840</v>
+      </c>
+      <c r="C6">
+        <v>8.1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6.3</v>
+      </c>
+      <c r="B7">
+        <v>850</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6.3</v>
+      </c>
+      <c r="B8">
+        <v>860</v>
+      </c>
+      <c r="C8">
+        <v>7.9</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6.2</v>
+      </c>
+      <c r="B9">
+        <v>860</v>
+      </c>
+      <c r="C9">
+        <v>7.8</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6.2</v>
+      </c>
+      <c r="B10">
+        <v>865</v>
+      </c>
+      <c r="C10">
+        <v>7.7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>790</v>
+      </c>
+      <c r="C11">
+        <v>8.5</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>795</v>
+      </c>
+      <c r="C12">
+        <v>8.4</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6.1</v>
+      </c>
+      <c r="B13">
+        <v>800</v>
+      </c>
+      <c r="C13">
+        <v>8.4</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6.2</v>
+      </c>
+      <c r="B14">
+        <v>810</v>
+      </c>
+      <c r="C14">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>6.3</v>
+      </c>
+      <c r="B15">
+        <v>820</v>
+      </c>
+      <c r="C15">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>6.3</v>
+      </c>
+      <c r="B16">
+        <v>830</v>
+      </c>
+      <c r="C16">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F210B8CE-835E-FD46-A636-E41911D82DC5}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3DCD7-E28A-B947-91E9-75F0CD39EC16}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -621,35 +815,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA8ABB4-3654-1443-BA27-845A6F240641}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B04D9FBA-A7E1-9B47-83F3-195C0ECD4B77}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F210B8CE-835E-FD46-A636-E41911D82DC5}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9AFE0D-20AE-8C4F-9881-9960F9203F3B}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -657,330 +941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3DCD7-E28A-B947-91E9-75F0CD39EC16}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB536F2-B6F5-5D4C-A150-E99119632D93}">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1000</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>800</v>
-      </c>
-      <c r="D2">
-        <v>8.5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1001</v>
-      </c>
-      <c r="B3">
-        <v>6.1</v>
-      </c>
-      <c r="C3">
-        <v>810</v>
-      </c>
-      <c r="D3">
-        <v>8.4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1002</v>
-      </c>
-      <c r="B4">
-        <v>6.1</v>
-      </c>
-      <c r="C4">
-        <v>820</v>
-      </c>
-      <c r="D4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1003</v>
-      </c>
-      <c r="B5">
-        <v>6.1</v>
-      </c>
-      <c r="C5">
-        <v>830</v>
-      </c>
-      <c r="D5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1004</v>
-      </c>
-      <c r="B6">
-        <v>6.2</v>
-      </c>
-      <c r="C6">
-        <v>840</v>
-      </c>
-      <c r="D6">
-        <v>8.1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1005</v>
-      </c>
-      <c r="B7">
-        <v>6.3</v>
-      </c>
-      <c r="C7">
-        <v>850</v>
-      </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1006</v>
-      </c>
-      <c r="B8">
-        <v>6.3</v>
-      </c>
-      <c r="C8">
-        <v>860</v>
-      </c>
-      <c r="D8">
-        <v>7.9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1007</v>
-      </c>
-      <c r="B9">
-        <v>6.2</v>
-      </c>
-      <c r="C9">
-        <v>860</v>
-      </c>
-      <c r="D9">
-        <v>7.8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1008</v>
-      </c>
-      <c r="B10">
-        <v>6.2</v>
-      </c>
-      <c r="C10">
-        <v>865</v>
-      </c>
-      <c r="D10">
-        <v>7.7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1009</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>790</v>
-      </c>
-      <c r="D11">
-        <v>8.5</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1010</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>795</v>
-      </c>
-      <c r="D12">
-        <v>8.4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1011</v>
-      </c>
-      <c r="B13">
-        <v>6.1</v>
-      </c>
-      <c r="C13">
-        <v>800</v>
-      </c>
-      <c r="D13">
-        <v>8.4</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1012</v>
-      </c>
-      <c r="B14">
-        <v>6.2</v>
-      </c>
-      <c r="C14">
-        <v>810</v>
-      </c>
-      <c r="D14">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1013</v>
-      </c>
-      <c r="B15">
-        <v>6.3</v>
-      </c>
-      <c r="C15">
-        <v>820</v>
-      </c>
-      <c r="D15">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1014</v>
-      </c>
-      <c r="B16">
-        <v>6.3</v>
-      </c>
-      <c r="C16">
-        <v>830</v>
-      </c>
-      <c r="D16">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA01E968-AB9B-6749-B752-3E77062917A3}">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -992,16 +953,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1015,7 +976,7 @@
         <v>8.5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1029,7 +990,7 @@
         <v>8.4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1043,7 +1004,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1057,7 +1018,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1071,7 +1032,7 @@
         <v>8.1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1085,7 +1046,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1099,7 +1060,7 @@
         <v>7.9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1113,7 +1074,7 @@
         <v>7.8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1127,7 +1088,7 @@
         <v>7.7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1141,7 +1102,7 @@
         <v>8.5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1155,7 +1116,7 @@
         <v>8.4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1169,7 +1130,7 @@
         <v>8.4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1183,7 +1144,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1197,7 +1158,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1211,7 +1172,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add seed lot function working
</commit_message>
<xml_diff>
--- a/SampleData/SampleData.xlsx
+++ b/SampleData/SampleData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/Documents/GitHub/Harvester/SampleData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3C6BB2-D56D-CB4F-98F8-90F66C95909D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BC295B-8965-FF40-9327-237BBC8136F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35140" yWindow="3040" windowWidth="29400" windowHeight="22660" activeTab="5" xr2:uid="{2FC47D8B-67C3-324E-B295-947C478D14E9}"/>
+    <workbookView xWindow="13140" yWindow="900" windowWidth="20300" windowHeight="22840" activeTab="1" xr2:uid="{2FC47D8B-67C3-324E-B295-947C478D14E9}"/>
   </bookViews>
   <sheets>
     <sheet name="SolutionReadings" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="136">
   <si>
     <t>PH</t>
   </si>
@@ -173,6 +173,282 @@
   </si>
   <si>
     <t>seedling_id</t>
+  </si>
+  <si>
+    <t>2022-04-16</t>
+  </si>
+  <si>
+    <t>2022-04-17</t>
+  </si>
+  <si>
+    <t>2022-04-18</t>
+  </si>
+  <si>
+    <t>2022-04-19</t>
+  </si>
+  <si>
+    <t>2022-04-20</t>
+  </si>
+  <si>
+    <t>2022-04-21</t>
+  </si>
+  <si>
+    <t>2022-04-22</t>
+  </si>
+  <si>
+    <t>2022-04-23</t>
+  </si>
+  <si>
+    <t>2022-04-24</t>
+  </si>
+  <si>
+    <t>2022-04-25</t>
+  </si>
+  <si>
+    <t>2022-04-26</t>
+  </si>
+  <si>
+    <t>2022-04-27</t>
+  </si>
+  <si>
+    <t>2022-04-28</t>
+  </si>
+  <si>
+    <t>2022-04-29</t>
+  </si>
+  <si>
+    <t>2022-04-30</t>
+  </si>
+  <si>
+    <t>Watermelon</t>
+  </si>
+  <si>
+    <t>Mini Love</t>
+  </si>
+  <si>
+    <t>Sugar Baby</t>
+  </si>
+  <si>
+    <t>ph</t>
+  </si>
+  <si>
+    <t>tds</t>
+  </si>
+  <si>
+    <t>1260-1680</t>
+  </si>
+  <si>
+    <t>Bean-Bush</t>
+  </si>
+  <si>
+    <t>Commodore Improved</t>
+  </si>
+  <si>
+    <t>Kentucky Wonder</t>
+  </si>
+  <si>
+    <t>Blue Lake 274</t>
+  </si>
+  <si>
+    <t>Pea</t>
+  </si>
+  <si>
+    <t>Dward White Sugar</t>
+  </si>
+  <si>
+    <t>Thomas Laxton</t>
+  </si>
+  <si>
+    <t>Wando</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>580-1260</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1400-1800</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>Lakeside</t>
+  </si>
+  <si>
+    <t>New Zeland</t>
+  </si>
+  <si>
+    <t>Nobel Giant</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>1260-1610</t>
+  </si>
+  <si>
+    <t>5.5-6.5</t>
+  </si>
+  <si>
+    <t>Lettuce</t>
+  </si>
+  <si>
+    <t>Iceberg</t>
+  </si>
+  <si>
+    <t>Green Oakleaf</t>
+  </si>
+  <si>
+    <t>Black Seeded Simpson</t>
+  </si>
+  <si>
+    <t>Salad Bowl Greens</t>
+  </si>
+  <si>
+    <t>Buttercrunch</t>
+  </si>
+  <si>
+    <t>White Boston</t>
+  </si>
+  <si>
+    <t>Little Gem</t>
+  </si>
+  <si>
+    <t>Four Seasons</t>
+  </si>
+  <si>
+    <t>Cimarron</t>
+  </si>
+  <si>
+    <t>Prizehead</t>
+  </si>
+  <si>
+    <t>Bronze Mignoette</t>
+  </si>
+  <si>
+    <t>Bibb</t>
+  </si>
+  <si>
+    <t>600-800</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Tiny Tim</t>
+  </si>
+  <si>
+    <t>Small Red Cherry</t>
+  </si>
+  <si>
+    <t>1400-3500</t>
+  </si>
+  <si>
+    <t>Herb</t>
+  </si>
+  <si>
+    <t>Cilantro</t>
+  </si>
+  <si>
+    <t>Chervil</t>
+  </si>
+  <si>
+    <t>Chives - Garlic</t>
+  </si>
+  <si>
+    <t>Basil - Sweet</t>
+  </si>
+  <si>
+    <t>Chives</t>
+  </si>
+  <si>
+    <t>Parsley - Curled</t>
+  </si>
+  <si>
+    <t>Parsley - Italian</t>
+  </si>
+  <si>
+    <t>Dill</t>
+  </si>
+  <si>
+    <t>Fennel</t>
+  </si>
+  <si>
+    <t>Mint</t>
+  </si>
+  <si>
+    <t>Peppermint</t>
+  </si>
+  <si>
+    <t>Lemon Mint</t>
+  </si>
+  <si>
+    <t>Lemon Balm</t>
+  </si>
+  <si>
+    <t>Lavender</t>
+  </si>
+  <si>
+    <t>Bergamot</t>
+  </si>
+  <si>
+    <t>Chamomile</t>
+  </si>
+  <si>
+    <t>Purple Coneflower</t>
+  </si>
+  <si>
+    <t>Catnip</t>
+  </si>
+  <si>
+    <t>700-1120</t>
+  </si>
+  <si>
+    <t>6-6.5</t>
+  </si>
+  <si>
+    <t>6.5-6.7</t>
+  </si>
+  <si>
+    <t>910-1260</t>
+  </si>
+  <si>
+    <t>also called French Parsley</t>
+  </si>
+  <si>
+    <t>5.5-6.0</t>
+  </si>
+  <si>
+    <t>560-1260</t>
+  </si>
+  <si>
+    <t>1400-1680</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>5.0-5.5</t>
+  </si>
+  <si>
+    <t>6.4-6.8</t>
+  </si>
+  <si>
+    <t>700-980</t>
+  </si>
+  <si>
+    <t>Everbearing</t>
+  </si>
+  <si>
+    <t>5.8-6.5</t>
   </si>
 </sst>
 </file>
@@ -540,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB536F2-B6F5-5D4C-A150-E99119632D93}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,6 +1051,216 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>800</v>
+      </c>
+      <c r="C17">
+        <v>8.5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6.1</v>
+      </c>
+      <c r="B18">
+        <v>810</v>
+      </c>
+      <c r="C18">
+        <v>8.4</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6.1</v>
+      </c>
+      <c r="B19">
+        <v>820</v>
+      </c>
+      <c r="C19">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>6.1</v>
+      </c>
+      <c r="B20">
+        <v>830</v>
+      </c>
+      <c r="C20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6.2</v>
+      </c>
+      <c r="B21">
+        <v>840</v>
+      </c>
+      <c r="C21">
+        <v>8.1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>6.3</v>
+      </c>
+      <c r="B22">
+        <v>850</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>6.3</v>
+      </c>
+      <c r="B23">
+        <v>860</v>
+      </c>
+      <c r="C23">
+        <v>7.9</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>6.2</v>
+      </c>
+      <c r="B24">
+        <v>860</v>
+      </c>
+      <c r="C24">
+        <v>7.8</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>6.2</v>
+      </c>
+      <c r="B25">
+        <v>865</v>
+      </c>
+      <c r="C25">
+        <v>7.7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>790</v>
+      </c>
+      <c r="C26">
+        <v>8.5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>795</v>
+      </c>
+      <c r="C27">
+        <v>8.4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>6.1</v>
+      </c>
+      <c r="B28">
+        <v>800</v>
+      </c>
+      <c r="C28">
+        <v>8.4</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>6.2</v>
+      </c>
+      <c r="B29">
+        <v>810</v>
+      </c>
+      <c r="C29">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>6.3</v>
+      </c>
+      <c r="B30">
+        <v>820</v>
+      </c>
+      <c r="C30">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>6.3</v>
+      </c>
+      <c r="B31">
+        <v>830</v>
+      </c>
+      <c r="C31">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -783,29 +1269,660 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D3DCD7-E28A-B947-91E9-75F0CD39EC16}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -818,7 +1935,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9AFE0D-20AE-8C4F-9881-9960F9203F3B}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>